<commit_message>
teensy adapter board updated to version 2 with…
 - bugfixes
 - reset controller
 - audio
 - swd debugger port
</commit_message>
<xml_diff>
--- a/v2/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/v2/teensy/teensy_3.6_pin_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/teensy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/v2/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4241A34-C5CA-2B48-8C45-AFBDDFB3922D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C5B844-24CF-164C-B54A-C3EE99F226BF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35240" windowHeight="29760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="208">
   <si>
     <t>Pin</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Maus SDIO</t>
   </si>
   <si>
-    <t>Bluetooth Uart</t>
-  </si>
-  <si>
     <t>V_BAT_FB</t>
   </si>
   <si>
@@ -351,12 +348,6 @@
     <t>RPi SPI Slave CS</t>
   </si>
   <si>
-    <t>WiFi / USB2Bot TX</t>
-  </si>
-  <si>
-    <t>WiFi / USB2Bot RX</t>
-  </si>
-  <si>
     <t>RPI_MOSI0</t>
   </si>
   <si>
@@ -381,12 +372,6 @@
     <t>TXD2</t>
   </si>
   <si>
-    <t>MLINKS_3V3</t>
-  </si>
-  <si>
-    <t>MRECHTS_3V3</t>
-  </si>
-  <si>
     <t>ABSTL_3V3</t>
   </si>
   <si>
@@ -420,9 +405,6 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>Reset Teensy via RPi</t>
-  </si>
-  <si>
     <t>MLINKS</t>
   </si>
   <si>
@@ -486,9 +468,6 @@
     <t>GPIO42 (CS)</t>
   </si>
   <si>
-    <t>PWM Erweiterung Motor</t>
-  </si>
-  <si>
     <t>PWM6</t>
   </si>
   <si>
@@ -579,9 +558,6 @@
     <t>A2/SCL0/PWM (TPM1)</t>
   </si>
   <si>
-    <t>I2C 2 (Ena, LED, LCD)</t>
-  </si>
-  <si>
     <t>A3/SDA0/PWM (TPM1)</t>
   </si>
   <si>
@@ -600,9 +576,6 @@
     <t>Erweiterung oder SPI CS</t>
   </si>
   <si>
-    <t>PWM_ERW</t>
-  </si>
-  <si>
     <t>MAUS_D_3V3</t>
   </si>
   <si>
@@ -618,9 +591,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>This work is licensed under the Creative Commons Attribution-ShareAlike 4.0 International License. To view a copy of this license, visit http://creativecommons.org/licenses/by-sa/4.0</t>
-  </si>
-  <si>
     <t>PWM1</t>
   </si>
   <si>
@@ -645,7 +615,43 @@
     <t>RPi SPI Slave SCK</t>
   </si>
   <si>
-    <t>I2C 0 oder Uart 3</t>
+    <t>I2C 0 (5V: Ena, LED, LCD)</t>
+  </si>
+  <si>
+    <t>PWM_ERW1</t>
+  </si>
+  <si>
+    <t>PWM_ERW2</t>
+  </si>
+  <si>
+    <t>PWM_ERW3</t>
+  </si>
+  <si>
+    <t>PWM Erweiterung 1 (Motor)</t>
+  </si>
+  <si>
+    <t>PWM Erweiterung 2 oder I2C 2</t>
+  </si>
+  <si>
+    <t>PWM Erweiterung 3 oder I2C 2</t>
+  </si>
+  <si>
+    <t>Wi-Fi oder USB2Bot TX</t>
+  </si>
+  <si>
+    <t>Wi-Fi oder USB2Bot RX</t>
+  </si>
+  <si>
+    <t>Reset Teensy</t>
+  </si>
+  <si>
+    <t>Audio Out</t>
+  </si>
+  <si>
+    <t>This work (excluding the teensy images) is licensed under the Creative Commons Attribution-ShareAlike 4.0 International License. To view a copy of this license, visit http://creativecommons.org/licenses/by-sa/4.0</t>
+  </si>
+  <si>
+    <t>AUDIO_OUT</t>
   </si>
 </sst>
 </file>
@@ -692,7 +698,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -749,12 +755,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -790,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -894,6 +894,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -902,7 +922,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -933,13 +953,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -949,21 +967,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1034,16 +1052,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1100,7 +1122,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9202615" y="4953699"/>
+          <a:off x="8948615" y="4953699"/>
           <a:ext cx="5783386" cy="5595049"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1262,6 +1284,234 @@
           <a:r>
             <a:rPr lang="de-DE" sz="900"/>
             <a:t>Sources: https://www.pjrc.com/teensy/card9a_rev1.pdf; https://www.pjrc.com/teensy/card9b_rev1.pdf</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Gerade Verbindung mit Pfeil 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD347F0B-5940-DC4A-ABF3-6F01D447B9EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9417050" y="8336844"/>
+          <a:ext cx="1320800" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>176388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>458611</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Gerade Verbindung mit Pfeil 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB57FE77-15D9-7F4D-8786-C76FFE109934}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9417050" y="8565444"/>
+          <a:ext cx="1328561" cy="1412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>645317</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57856</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1035155" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Textfeld 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA0433A7-26E5-C44F-AD45-96A91F9F2950}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8450932" y="8469164"/>
+          <a:ext cx="1035155" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>MKL02 DC (14)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>645317</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19757</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1046761" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Textfeld 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED764666-7175-E140-8077-2D3B6CF2BFCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8450932" y="8225911"/>
+          <a:ext cx="1046761" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>MKL02 DD (16)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1537,10 +1787,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1557,41 +1807,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="75" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="62" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" s="62" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="63" t="s">
+      <c r="E1" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="63" t="s">
-        <v>97</v>
+      <c r="L1" s="61" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1601,24 +1851,24 @@
       <c r="B2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="22" t="s">
+      <c r="D2" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="82"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -1627,56 +1877,56 @@
       <c r="B3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="45" t="s">
+      <c r="D3" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="83"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="50" t="s">
+      <c r="G4" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="57" t="s">
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="55" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1684,129 +1934,133 @@
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="71" t="s">
+      <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="H5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="80" t="s">
+      <c r="G6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="H6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="46" t="s">
+      <c r="B7" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" s="46" t="s">
+      <c r="F7" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="I7" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="47" t="s">
+      <c r="B8" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="H8" s="47" t="s">
+      <c r="F8" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56" t="s">
+      <c r="I8" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1814,95 +2068,91 @@
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="E9" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="55" t="s">
-        <v>56</v>
-      </c>
+      <c r="B9" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>205</v>
-      </c>
-      <c r="E10" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="58" t="s">
-        <v>56</v>
-      </c>
+      <c r="B10" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="79"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="I11" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55" t="s">
+      <c r="B11" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11" s="77"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1910,27 +2160,27 @@
       <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="I12" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58" t="s">
+      <c r="B12" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="79"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1938,27 +2188,27 @@
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="79"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55" t="s">
+      <c r="D13" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="77"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1966,27 +2216,27 @@
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56" t="s">
+      <c r="D14" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="78"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1998,49 +2248,49 @@
         <v>8</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="57"/>
+        <v>102</v>
+      </c>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="55"/>
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16" s="79"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55" t="s">
+      <c r="B16" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="77"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2048,27 +2298,27 @@
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56" t="s">
+      <c r="B17" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="78"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2076,161 +2326,161 @@
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="79" t="s">
+      <c r="B18" s="89" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="I18" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
+      <c r="F18" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="69" t="s">
+      <c r="B19" s="89" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="69" t="s">
-        <v>132</v>
-      </c>
-      <c r="G19" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="H19" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="I19" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
+      <c r="F19" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="79" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="46" t="s">
+      <c r="G20" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="H20" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
+      <c r="I20" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" s="47" t="s">
+      <c r="G21" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="47" t="s">
+      <c r="H21" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
+      <c r="I21" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C22" s="22" t="s">
+      <c r="B22" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="79" t="s">
+      <c r="E22" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="H22" s="46" t="s">
+      <c r="F22" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="55" t="s">
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2238,33 +2488,33 @@
       <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="69" t="s">
+      <c r="E23" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="69" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="H23" s="79" t="s">
+      <c r="F23" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L23" s="55" t="s">
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2272,33 +2522,33 @@
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="79" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="G24" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="46" t="s">
+      <c r="E24" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L24" s="55" t="s">
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2306,33 +2556,33 @@
       <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="C25" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="H25" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L25" s="56" t="s">
+      <c r="B25" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2340,79 +2590,79 @@
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="79"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="22" t="s">
+      <c r="E26" s="77"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
+      <c r="I26" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="80"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="45" t="s">
+      <c r="E27" s="78"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
+      <c r="I27" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="79"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="22" t="s">
+      <c r="E28" s="77"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55" t="s">
+      <c r="I28" s="53"/>
+      <c r="J28" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2420,27 +2670,27 @@
       <c r="A29" s="6">
         <v>27</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="45" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="45" t="s">
+      <c r="C29" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="80"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="45" t="s">
+      <c r="E29" s="78"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56" t="s">
+      <c r="I29" s="54"/>
+      <c r="J29" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2448,7 +2698,7 @@
       <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="28" t="s">
         <v>74</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -2457,554 +2707,578 @@
       <c r="D30" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="76"/>
-      <c r="F30" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="50"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="48"/>
       <c r="H30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
+      <c r="I30" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>29</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="E31" s="79" t="s">
+      <c r="B31" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="F31" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="H31" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="I31" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
+      <c r="H31" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="E32" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="F32" s="47" t="s">
+      <c r="B32" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="47" t="s">
+      <c r="G32" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="I32" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H32" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="E33" s="86"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="22" t="s">
+      <c r="D33" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="84"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I33" s="53"/>
+      <c r="J33" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C34" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="87"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="45" t="s">
+      <c r="D34" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="85"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I34" s="54"/>
+      <c r="J34" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="79"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="77"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L35" s="53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="D36" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="80"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B36" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="78"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="F37" s="46" t="s">
+      <c r="B37" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="H37" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="I37" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="55"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G37" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="I37" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="53"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D38" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="F38" s="47" t="s">
+      <c r="B38" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="I38" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="56"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G38" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="H38" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="54"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="66"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="46" t="s">
+      <c r="B39" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="E39" s="86" t="s">
+      <c r="D39" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" s="84" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="F39" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="G39" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="H39" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="I39" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="55"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H39" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="V39" s="66"/>
+      <c r="W39" s="66"/>
+      <c r="X39" s="66"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="46" t="s">
+      <c r="B40" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" s="72" t="s">
+      <c r="D40" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="F40" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="G40" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="H40" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="I40" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="55"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H40" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="I40" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="66"/>
+      <c r="X40" s="66"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="D41" s="45" t="s">
+      <c r="C41" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="80" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E41" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
+      <c r="V41" s="66"/>
+      <c r="W41" s="66"/>
+      <c r="X41" s="66"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42" s="84"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" s="86"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L42" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I42" s="53"/>
+      <c r="J42" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="V42" s="66"/>
+      <c r="W42" s="66"/>
+      <c r="X42" s="66"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="52" t="s">
+      <c r="D43" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="87"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="45" t="s">
+      <c r="E43" s="85"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L43" s="56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L43" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="V43" s="66"/>
+      <c r="W43" s="66"/>
+      <c r="X43" s="66"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>40</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="79" t="s">
-        <v>135</v>
-      </c>
-      <c r="F44" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L44" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D44" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="V44" s="66"/>
+      <c r="W44" s="66"/>
+      <c r="X44" s="66"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>41</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="68" t="s">
+      <c r="D45" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="68" t="s">
+      <c r="F45" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="G45" s="68"/>
-      <c r="H45" s="71" t="s">
+      <c r="G45" s="66"/>
+      <c r="H45" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L45" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L45" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="V45" s="66"/>
+      <c r="W45" s="66"/>
+      <c r="X45" s="66"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>42</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="78" t="s">
+      <c r="D46" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="45" t="s">
+      <c r="F46" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L46" s="56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G46" s="43"/>
+      <c r="H46" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>43</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="51" t="s">
+      <c r="D47" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="84"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="22" t="s">
+      <c r="E47" s="82"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L47" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L47" s="53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>44</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="51" t="s">
+      <c r="D48" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="E48" s="84"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="22" t="s">
+      <c r="E48" s="82"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L48" s="55" t="s">
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L48" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3012,27 +3286,27 @@
       <c r="A49" s="8">
         <v>45</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="51" t="s">
+      <c r="D49" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="84"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="22" t="s">
+      <c r="E49" s="82"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L49" s="55" t="s">
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L49" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3040,27 +3314,27 @@
       <c r="A50" s="9">
         <v>46</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="52" t="s">
+      <c r="D50" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="85"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="45" t="s">
+      <c r="E50" s="83"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="I50" s="56"/>
-      <c r="J50" s="56"/>
-      <c r="K50" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L50" s="56" t="s">
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
+      <c r="K50" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3068,27 +3342,27 @@
       <c r="A51" s="8">
         <v>47</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="51" t="s">
+      <c r="D51" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="E51" s="84"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="22" t="s">
+      <c r="E51" s="82"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L51" s="55" t="s">
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L51" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3096,27 +3370,27 @@
       <c r="A52" s="6">
         <v>48</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="D52" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="85"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="45" t="s">
+      <c r="E52" s="83"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="I52" s="45"/>
-      <c r="J52" s="45"/>
-      <c r="K52" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L52" s="56" t="s">
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L52" s="54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3124,29 +3398,29 @@
       <c r="A53" s="5">
         <v>49</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="C53" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="73" t="s">
+      <c r="D53" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22" t="s">
+      <c r="E53" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
-      <c r="K53" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L53" s="55" t="s">
+      <c r="I53" s="53"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L53" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3154,55 +3428,55 @@
       <c r="A54" s="6">
         <v>50</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="47" t="s">
+      <c r="C54" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="D54" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="78"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45" t="s">
+      <c r="E54" s="76"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I54" s="56"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L54" s="56" t="s">
+      <c r="I54" s="54"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L54" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="77">
+      <c r="A55" s="75">
         <v>51</v>
       </c>
-      <c r="B55" s="89" t="s">
-        <v>178</v>
-      </c>
-      <c r="C55" s="64" t="s">
+      <c r="B55" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="64" t="s">
+      <c r="D55" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="E55" s="78"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="50" t="s">
+      <c r="E55" s="76"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="I55" s="65"/>
-      <c r="J55" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="K55" s="65"/>
-      <c r="L55" s="65" t="s">
+      <c r="I55" s="63"/>
+      <c r="J55" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3210,139 +3484,139 @@
       <c r="A56" s="5">
         <v>52</v>
       </c>
-      <c r="B56" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="E56" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="I56" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J56" s="55"/>
-      <c r="K56" s="55"/>
-      <c r="L56" s="55"/>
+      <c r="B56" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="I56" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>53</v>
       </c>
-      <c r="B57" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="D57" s="46" t="s">
+      <c r="B57" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="78" t="s">
-        <v>142</v>
-      </c>
-      <c r="F57" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="I57" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J57" s="55"/>
-      <c r="K57" s="88"/>
-      <c r="L57" s="55"/>
+      <c r="E57" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="I57" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J57" s="53"/>
+      <c r="K57" s="86"/>
+      <c r="L57" s="53"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>54</v>
       </c>
-      <c r="B58" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="C58" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E58" s="71"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22" t="s">
+      <c r="B58" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C58" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="69"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I58" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="55"/>
+      <c r="I58" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J58" s="53"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="53"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>55</v>
       </c>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C59" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="45" t="s">
+      <c r="D59" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E59" s="78"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45" t="s">
+      <c r="E59" s="76"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="I59" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J59" s="56"/>
-      <c r="K59" s="56"/>
-      <c r="L59" s="56"/>
+      <c r="I59" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J59" s="54"/>
+      <c r="K59" s="54"/>
+      <c r="L59" s="54"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>56</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E60" s="71"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="I60" s="55"/>
-      <c r="J60" s="55"/>
-      <c r="K60" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L60" s="55" t="s">
+      <c r="E60" s="69"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L60" s="53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3350,191 +3624,191 @@
       <c r="A61" s="6">
         <v>57</v>
       </c>
-      <c r="B61" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="45" t="s">
+      <c r="B61" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="E61" s="78"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="I61" s="56"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L61" s="56" t="s">
+      <c r="D61" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" s="76"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L61" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="77" t="s">
+      <c r="A62" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="83" t="s">
+      <c r="B62" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" s="22" t="s">
+      <c r="C62" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="82"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64" t="s">
+      <c r="E62" s="80"/>
+      <c r="F62" s="62"/>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="I62" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="J62" s="65"/>
-      <c r="K62" s="65"/>
-      <c r="L62" s="66"/>
+      <c r="I62" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="J62" s="63"/>
+      <c r="K62" s="63"/>
+      <c r="L62" s="64"/>
     </row>
     <row r="63" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="27" t="s">
+      <c r="B63" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D63" s="45" t="s">
+      <c r="C63" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="80"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47" t="s">
+      <c r="E63" s="78"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="I63" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="60"/>
+      <c r="I63" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J63" s="54"/>
+      <c r="K63" s="54"/>
+      <c r="L63" s="58"/>
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="67" t="s">
-        <v>192</v>
-      </c>
-      <c r="B64" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="D64" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="E64" s="86"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="I64" s="46"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L64" s="59" t="s">
+      <c r="A64" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E64" s="84"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="I64" s="44"/>
+      <c r="J64" s="44"/>
+      <c r="K64" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L64" s="57" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D65" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" s="87"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="L65" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65" s="85"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="I65" s="54"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L65" s="58" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B66" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="D66" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="E66" s="76"/>
-      <c r="F66" s="50"/>
-      <c r="G66" s="50"/>
-      <c r="H66" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="I66" s="57"/>
-      <c r="J66" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="K66" s="57"/>
-      <c r="L66" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D66" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" s="74"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="I66" s="55"/>
+      <c r="J66" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K66" s="55"/>
+      <c r="L66" s="55" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C67" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="D67" s="50" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="76"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="I67" s="57"/>
-      <c r="J67" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="K67" s="57"/>
-      <c r="L67" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="E67" s="74"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="I67" s="55"/>
+      <c r="J67" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K67" s="55"/>
+      <c r="L67" s="55" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3554,8 +3828,8 @@
       <c r="L70" s="3"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="90" t="s">
-        <v>196</v>
+      <c r="A71" s="88" t="s">
+        <v>206</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -3563,65 +3837,65 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="B72" s="68"/>
-      <c r="C72" s="68"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
-      <c r="I72" s="70"/>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="68"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-      <c r="B73" s="68"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
-      <c r="I73" s="70"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="68"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
-      <c r="B74" s="68"/>
-      <c r="C74" s="69"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="69"/>
-      <c r="F74" s="69"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="69"/>
-      <c r="I74" s="70"/>
+      <c r="B74" s="66"/>
+      <c r="C74" s="67"/>
+      <c r="D74" s="72"/>
+      <c r="E74" s="67"/>
+      <c r="F74" s="67"/>
+      <c r="G74" s="67"/>
+      <c r="H74" s="67"/>
+      <c r="I74" s="68"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
-      <c r="B75" s="68"/>
-      <c r="C75" s="69"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
-      <c r="I75" s="70"/>
+      <c r="B75" s="66"/>
+      <c r="C75" s="67"/>
+      <c r="D75" s="72"/>
+      <c r="E75" s="67"/>
+      <c r="F75" s="67"/>
+      <c r="G75" s="67"/>
+      <c r="H75" s="67"/>
+      <c r="I75" s="68"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="68"/>
+      <c r="B76" s="66"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="66"/>
+      <c r="H76" s="66"/>
+      <c r="I76" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.19685039370078741" footer="3.937007874015748E-2"/>

</xml_diff>

<commit_message>
ct-bot v2 schematic updated
- optional current measurements added to mainboard
 - schematic drafts for sensor boards
 - pin mapping sheet updated (i2c-bus mapping)
</commit_message>
<xml_diff>
--- a/v2/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/v2/teensy/teensy_3.6_pin_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/v2/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A502718-947E-0943-9CF2-E554D403D23A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A2F9F-C0AC-5C4C-936D-353030F76392}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="47420" windowHeight="30920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="313">
   <si>
     <t>Pin</t>
   </si>
@@ -870,9 +870,6 @@
     <t>PWM_ERW_5</t>
   </si>
   <si>
-    <t>I2C 0 (5V: Ena, LED)</t>
-  </si>
-  <si>
     <t>SERVO_1_PWM</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>SCL3/PWM (FTM3)</t>
   </si>
   <si>
-    <t>I2C 3 oder PWM Erweiterung</t>
-  </si>
-  <si>
     <t>Servo 3</t>
   </si>
   <si>
@@ -919,9 +913,6 @@
   </si>
   <si>
     <t>SERVO_3_PWM</t>
-  </si>
-  <si>
-    <t>Erweiterung (evtl. SCHRANKE)</t>
   </si>
   <si>
     <t>PWM Erweiterung 1</t>
@@ -1330,6 +1321,12 @@
       </rPr>
       <t>Rest ist noch zu überprüfen</t>
     </r>
+  </si>
+  <si>
+    <t>I2C 0 (5V: Sensoren, Ena)</t>
+  </si>
+  <si>
+    <t>I2C 3 (5V: LEDs, ENA CNY70)</t>
   </si>
 </sst>
 </file>
@@ -2721,8 +2718,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2854,7 +2851,7 @@
         <v>276</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E5" s="40"/>
       <c r="F5" s="40"/>
@@ -2876,10 +2873,10 @@
         <v>153</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
@@ -2901,7 +2898,7 @@
         <v>55</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>12</v>
@@ -2924,7 +2921,7 @@
         <v>195</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>13</v>
@@ -2952,7 +2949,7 @@
         <v>237</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="40" t="s">
@@ -2975,7 +2972,7 @@
         <v>238</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="43" t="s">
@@ -3092,7 +3089,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>78</v>
@@ -3140,7 +3137,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="97" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>259</v>
@@ -3163,13 +3160,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="88" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>235</v>
       </c>
       <c r="D18" s="56" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
@@ -3188,13 +3185,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="95" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>236</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
@@ -3262,10 +3259,10 @@
         <v>204</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
@@ -3287,10 +3284,10 @@
         <v>206</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
@@ -3360,7 +3357,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>25</v>
@@ -3382,13 +3379,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C27" s="82" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
@@ -3519,7 +3516,7 @@
         <v>245</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
@@ -3689,7 +3686,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C39" s="49" t="s">
         <v>253</v>
@@ -3717,7 +3714,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C40" s="32" t="s">
         <v>254</v>
@@ -3771,7 +3768,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>76</v>
@@ -3799,7 +3796,7 @@
         <v>7</v>
       </c>
       <c r="B43" s="100" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C43" s="30" t="s">
         <v>255</v>
@@ -3978,8 +3975,8 @@
       <c r="C50" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="D50" s="82" t="s">
-        <v>294</v>
+      <c r="D50" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="E50" s="41"/>
       <c r="F50" s="41"/>
@@ -3990,7 +3987,7 @@
         <v>26</v>
       </c>
       <c r="I50" s="64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -4004,7 +4001,7 @@
         <v>265</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E51" s="40"/>
       <c r="F51" s="40"/>
@@ -4029,7 +4026,7 @@
         <v>266</v>
       </c>
       <c r="D52" s="37" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E52" s="30"/>
       <c r="F52" s="30"/>
@@ -4204,7 +4201,7 @@
         <v>156</v>
       </c>
       <c r="L57" s="147" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="M57" s="147"/>
       <c r="N57" s="110"/>
@@ -4240,7 +4237,7 @@
         <v>157</v>
       </c>
       <c r="L58" s="148" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="M58" s="148"/>
       <c r="N58" s="72" t="s">
@@ -4293,22 +4290,20 @@
         <v>56</v>
       </c>
       <c r="B60" s="89" t="s">
-        <v>285</v>
-      </c>
-      <c r="C60" s="60" t="s">
+        <v>284</v>
+      </c>
+      <c r="C60" s="31" t="s">
         <v>272</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="40"/>
       <c r="G60" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H60" s="40" t="s">
-        <v>26</v>
-      </c>
+      <c r="H60" s="40"/>
       <c r="I60" s="62" t="s">
         <v>136</v>
       </c>
@@ -4316,7 +4311,7 @@
         <v>162</v>
       </c>
       <c r="L60" s="149" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="M60" s="149"/>
       <c r="N60" s="73"/>
@@ -4327,22 +4322,20 @@
         <v>57</v>
       </c>
       <c r="B61" s="90" t="s">
-        <v>286</v>
-      </c>
-      <c r="C61" s="82" t="s">
+        <v>285</v>
+      </c>
+      <c r="C61" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="D61" s="30" t="s">
-        <v>287</v>
+      <c r="D61" s="10" t="s">
+        <v>312</v>
       </c>
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
       <c r="G61" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H61" s="41" t="s">
-        <v>26</v>
-      </c>
+      <c r="H61" s="41"/>
       <c r="I61" s="64" t="s">
         <v>137</v>
       </c>
@@ -4358,7 +4351,7 @@
         <v>10</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>14</v>
@@ -4391,7 +4384,7 @@
         <v>11</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D63" s="30" t="s">
         <v>15</v>
@@ -4654,7 +4647,7 @@
     <row r="70" spans="1:17" ht="16" customHeight="1">
       <c r="A70" s="136"/>
       <c r="B70" s="139" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C70" s="140"/>
       <c r="D70" s="140"/>

</xml_diff>

<commit_message>
pin mapping sheet updated: fix for missing line
</commit_message>
<xml_diff>
--- a/v2/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/v2/teensy/teensy_3.6_pin_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/v2/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A2F9F-C0AC-5C4C-936D-353030F76392}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB534C1-C5BC-F34A-906D-24BC919D60FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="47420" windowHeight="30920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2718,9 +2718,7 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4327,7 +4325,7 @@
       <c r="C61" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="30" t="s">
         <v>312</v>
       </c>
       <c r="E61" s="41"/>

</xml_diff>

<commit_message>
pin mapping table updated after further testing
</commit_message>
<xml_diff>
--- a/v2/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/v2/teensy/teensy_3.6_pin_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/v2/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FBAB97-BE71-0D49-BEFA-56E314E06A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F4461-DA40-994B-9DE6-C7AE8519F6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9240" yWindow="460" windowWidth="42460" windowHeight="28460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="318">
   <si>
     <t>Pin</t>
   </si>
@@ -961,6 +961,33 @@
   </si>
   <si>
     <t>PWM Erweiterung 1/2</t>
+  </si>
+  <si>
+    <t>I2C 0 (5V: Sensoren, Ena)</t>
+  </si>
+  <si>
+    <t>I2C 3 (5V: LEDs, ENA CNY70)</t>
+  </si>
+  <si>
+    <t>Signale</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>AGND</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Servo 5 oder SPI0 CS 2</t>
+  </si>
+  <si>
+    <t>Servo 4 oder SPI0 CS 3</t>
+  </si>
+  <si>
+    <t>I2C 5V</t>
   </si>
   <si>
     <r>
@@ -973,7 +1000,15 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Textkörper)"/>
       </rPr>
-      <t>Performance Nachteil von SPI 1 checken</t>
+      <t xml:space="preserve">Performance Nachteil von SPI 1 checken
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>- Distanzsensoren über I2C (z.B. VL53L0X)</t>
     </r>
     <r>
       <rPr>
@@ -984,8 +1019,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-- SCHRANKE Transportfachüberwachung: evtl. über I2C, abhängig vom gewählten Sensor, evtl. VCNL4010
-- Distanzsensoren über I2C (z.B. VL53L0X)
+- Transportfachüberwachung über I2C (z.B. VL6180X)
 - Maussensor bisher nicht berücksichtigt, da aktuell unklar, ob verfügbar. Evtl. an SPI 2 anschließen
 - PWM auf alternativen Pin-Funktionen gelb markiert, unklar ob möglich, da kein Treiber-Support (25, 56, 57)
 - Verfügbare </t>
@@ -1199,25 +1233,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)"/>
-      </rPr>
-      <t>zu klären: Gibt es Unterschiede zwischen den I2C-Controllern?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
 - Verfügbare </t>
     </r>
@@ -1316,36 +1331,12 @@
       <t>Rest ist noch zu überprüfen</t>
     </r>
   </si>
-  <si>
-    <t>I2C 0 (5V: Sensoren, Ena)</t>
-  </si>
-  <si>
-    <t>I2C 3 (5V: LEDs, ENA CNY70)</t>
-  </si>
-  <si>
-    <t>Signale</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>AGND</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>Servo 5 oder SPI0 CS 2</t>
-  </si>
-  <si>
-    <t>Servo 4 oder SPI0 CS 3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1404,6 +1395,10 @@
       <i/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
@@ -2959,7 +2954,7 @@
         <v>237</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="40" t="s">
@@ -2982,7 +2977,7 @@
         <v>238</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="43" t="s">
@@ -3272,7 +3267,7 @@
         <v>288</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
@@ -3297,7 +3292,7 @@
         <v>287</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
@@ -4103,7 +4098,7 @@
       <c r="N54" s="102"/>
       <c r="O54" s="80"/>
       <c r="S54" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T54">
         <v>63</v>
@@ -4148,7 +4143,7 @@
       </c>
       <c r="Q55" s="52"/>
       <c r="S55" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T55">
         <v>1</v>
@@ -4193,7 +4188,7 @@
       </c>
       <c r="Q56" s="52"/>
       <c r="S56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T56">
         <v>1</v>
@@ -4235,7 +4230,7 @@
       <c r="Q57" s="52"/>
       <c r="R57" s="53"/>
       <c r="S57" s="53" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T57">
         <v>1</v>
@@ -4278,10 +4273,11 @@
       <c r="O58" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="S58" s="53"/>
+      <c r="S58" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="T58">
-        <f>SUM(T54:T57)</f>
-        <v>66</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -4321,6 +4317,10 @@
       <c r="O59" s="112" t="s">
         <v>170</v>
       </c>
+      <c r="T59">
+        <f>SUM(T54:T58)</f>
+        <v>68</v>
+      </c>
     </row>
     <row r="60" spans="1:20">
       <c r="A60" s="130">
@@ -4333,7 +4333,7 @@
         <v>272</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="40"/>
@@ -4365,7 +4365,7 @@
         <v>273</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
@@ -4684,7 +4684,7 @@
     <row r="70" spans="1:17" ht="16" customHeight="1">
       <c r="A70" s="136"/>
       <c r="B70" s="139" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="C70" s="140"/>
       <c r="D70" s="140"/>

</xml_diff>

<commit_message>
ct-Bot v2 prototype test boards updated/added
Simplified mainboard, teensy mcu board, and sensor boards are very early prototypes just for development and testing.
</commit_message>
<xml_diff>
--- a/v2/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/v2/teensy/teensy_3.6_pin_mapping.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/v2/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F4461-DA40-994B-9DE6-C7AE8519F6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9706C5-D95C-7749-832B-F5BE5DEFA0F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="460" windowWidth="42460" windowHeight="28460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="29080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$Q$82</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$U$82</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="400">
   <si>
     <t>Pin</t>
   </si>
@@ -1330,6 +1330,252 @@
       </rPr>
       <t>Rest ist noch zu überprüfen</t>
     </r>
+  </si>
+  <si>
+    <t>CS0</t>
+  </si>
+  <si>
+    <t>PWM/SCK0</t>
+  </si>
+  <si>
+    <t>A2/RX4/SCL1</t>
+  </si>
+  <si>
+    <t>A3/TX4/SDA1</t>
+  </si>
+  <si>
+    <t>A6/TX5</t>
+  </si>
+  <si>
+    <t>A7/RX5</t>
+  </si>
+  <si>
+    <t>A12/MOSI1</t>
+  </si>
+  <si>
+    <t>A13/SCK1</t>
+  </si>
+  <si>
+    <t>GPIO30</t>
+  </si>
+  <si>
+    <t>GPIO31</t>
+  </si>
+  <si>
+    <t>GPIO32</t>
+  </si>
+  <si>
+    <t>Funktion Teensy 4.0</t>
+  </si>
+  <si>
+    <t>SPI 0 Master CS 0</t>
+  </si>
+  <si>
+    <t>PWM (F: 2, 1)</t>
+  </si>
+  <si>
+    <t>PWM (F: 2, 0)</t>
+  </si>
+  <si>
+    <t>PWM (F: 4, 2)</t>
+  </si>
+  <si>
+    <t>TX1/PWM (F: 1, 0)</t>
+  </si>
+  <si>
+    <t>RX1/PWM (F: 1, 1)</t>
+  </si>
+  <si>
+    <t>PWM (F: 2, 2)</t>
+  </si>
+  <si>
+    <t>RX2/PWM (F: 1, 3)</t>
+  </si>
+  <si>
+    <t>TX2/PWM (F: 1, 3)</t>
+  </si>
+  <si>
+    <t>A0/TX3/PWM (Q: 3, 2)</t>
+  </si>
+  <si>
+    <t>A1/RX3/PWM (Q: 3, 3)</t>
+  </si>
+  <si>
+    <t>A4/SDA0/PWM (Q: 3, 1)</t>
+  </si>
+  <si>
+    <t>A5/SCL0/PWM (Q, 3, 0)</t>
+  </si>
+  <si>
+    <t>A8/PWM (F: 4, 0)</t>
+  </si>
+  <si>
+    <t>A9/PWM (F: 4, 1)</t>
+  </si>
+  <si>
+    <t>A10/TX6/SCL2/PWM (F: 1, 2)</t>
+  </si>
+  <si>
+    <t>A11/RX6/SDA2/PWM (F: 1, 3)</t>
+  </si>
+  <si>
+    <t>RX7/PWM (F: 3, 1)</t>
+  </si>
+  <si>
+    <t>TX7/PWM (F: 3, 1)</t>
+  </si>
+  <si>
+    <t>GPIO33/PWM (F: 2, 0)</t>
+  </si>
+  <si>
+    <t>BPS Sensor?</t>
+  </si>
+  <si>
+    <t>I2C 1 (5V: LEDs, ENA CNY70)</t>
+  </si>
+  <si>
+    <t>SPI Master CS / Display BL PWM</t>
+  </si>
+  <si>
+    <t>Verwendung Teensy 4.0</t>
+  </si>
+  <si>
+    <t>Uart 5 (WiFi) TX</t>
+  </si>
+  <si>
+    <t>Uart 5 (WiFi) RX</t>
+  </si>
+  <si>
+    <t>Uart 1 (RPi) RX</t>
+  </si>
+  <si>
+    <t>Uart 1 (RPi) TX</t>
+  </si>
+  <si>
+    <t>Funktion Teensy 3.2</t>
+  </si>
+  <si>
+    <t>RX1</t>
+  </si>
+  <si>
+    <t>TX1</t>
+  </si>
+  <si>
+    <t>RX3/MOSI</t>
+  </si>
+  <si>
+    <t>TX3/MISO</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>A0/SCK</t>
+  </si>
+  <si>
+    <t>A1/CS</t>
+  </si>
+  <si>
+    <t>A2/SCL0</t>
+  </si>
+  <si>
+    <t>A3/SDA0</t>
+  </si>
+  <si>
+    <t>GPIO24</t>
+  </si>
+  <si>
+    <t>A15/RX2</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18/SCL1</t>
+  </si>
+  <si>
+    <t>A19/SDA1</t>
+  </si>
+  <si>
+    <t>A20/TX2</t>
+  </si>
+  <si>
+    <t>GPIO33</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14/DAC</t>
+  </si>
+  <si>
+    <t>Verwendung Teensy 3.2</t>
+  </si>
+  <si>
+    <t>PWM (FTM1)</t>
+  </si>
+  <si>
+    <t>TX1/PWM (FTM0)</t>
+  </si>
+  <si>
+    <t>RX2/CS/PWM (FTM0)</t>
+  </si>
+  <si>
+    <t>TX2/CS/PWM (FTM0)</t>
+  </si>
+  <si>
+    <t>A6/CS/PWM (FTM0)</t>
+  </si>
+  <si>
+    <t>A7/RX1/CS/PWM (FTM0)</t>
+  </si>
+  <si>
+    <t>PWM (FTM2)</t>
+  </si>
+  <si>
+    <t>PWM (FTM0)/CS</t>
+  </si>
+  <si>
+    <t>A8/PWM (FTM0)/CS</t>
+  </si>
+  <si>
+    <t>A9/PWM (FTM0)/CS</t>
+  </si>
+  <si>
+    <t>SPI 0 Master CS 4</t>
+  </si>
+  <si>
+    <t>SPI 0 Master CS 5</t>
+  </si>
+  <si>
+    <t>GPIO2/CS</t>
+  </si>
+  <si>
+    <t>Uart 2 RX</t>
+  </si>
+  <si>
+    <t>Uart 2 TX</t>
+  </si>
+  <si>
+    <t>SPI Master CS 4</t>
+  </si>
+  <si>
+    <t>SPI Master CS 5</t>
+  </si>
+  <si>
+    <t>BPS oder Servo 4 oder SPI0 CS 3</t>
   </si>
 </sst>
 </file>
@@ -1755,7 +2001,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1782,7 +2028,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1907,7 +2152,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -2003,6 +2247,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2115,7 +2386,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>502278</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>102584</xdr:rowOff>
@@ -2174,13 +2445,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>18943</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>115135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>39078</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>134752</xdr:rowOff>
@@ -2198,8 +2469,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8039481" y="115135"/>
-          <a:ext cx="6887905" cy="10277309"/>
+          <a:off x="8045343" y="115135"/>
+          <a:ext cx="6886602" cy="10179617"/>
           <a:chOff x="8034884" y="115135"/>
           <a:chExt cx="6878135" cy="10104911"/>
         </a:xfrm>
@@ -2723,2169 +2994,2784 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U81"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="137" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="135" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="66" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="3" max="6" width="29.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="J1" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="K1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="L1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="M1" s="60" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="130">
+    <row r="2" spans="1:13">
+      <c r="A2" s="128">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="90" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>356</v>
+      </c>
+      <c r="E2" s="151" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" s="90" t="s">
+        <v>356</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="H2" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="62" t="s">
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="130">
+    <row r="3" spans="1:13">
+      <c r="A3" s="128">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="91" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>357</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>360</v>
+      </c>
+      <c r="F3" s="91" t="s">
+        <v>357</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="H3" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="61" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="D4" s="149" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="H4" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="40"/>
+      <c r="J4" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="63" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="130">
+    <row r="5" spans="1:13">
+      <c r="A5" s="128">
         <v>3</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="149" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="H5" s="30" t="s">
         <v>299</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="61" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="130">
+    <row r="6" spans="1:13">
+      <c r="A6" s="128">
         <v>4</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="H6" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="61" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="130">
+    <row r="7" spans="1:13">
+      <c r="A7" s="128">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="H7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="62" t="s">
+      <c r="I7" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="61" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="130">
+    <row r="9" spans="1:13">
+      <c r="A9" s="128">
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="150" t="s">
+        <v>337</v>
+      </c>
+      <c r="D9" s="150" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" s="160" t="s">
+        <v>361</v>
+      </c>
+      <c r="F9" s="150" t="s">
+        <v>355</v>
+      </c>
+      <c r="G9" s="55" t="s">
         <v>237</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="62" t="s">
+      <c r="I9" s="39"/>
+      <c r="J9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="61" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="161" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" s="155" t="s">
+        <v>354</v>
+      </c>
+      <c r="G10" s="162" t="s">
         <v>238</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="68" t="s">
+      <c r="I10" s="42"/>
+      <c r="J10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="67" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="130">
+    <row r="11" spans="1:13">
+      <c r="A11" s="128">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="146" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="G11" s="53" t="s">
         <v>239</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="62" t="s">
+      <c r="I11" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="61" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="97" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="163" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="H12" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="67" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="130">
+    <row r="13" spans="1:13">
+      <c r="A13" s="128">
         <v>11</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="H13" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="39"/>
+      <c r="J13" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="61" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="H14" s="81" t="s">
         <v>215</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="40"/>
+      <c r="J14" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="131">
+    <row r="15" spans="1:13">
+      <c r="A15" s="129">
         <v>13</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="96" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="96" t="s">
+        <v>365</v>
+      </c>
+      <c r="F15" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="67" t="s">
+      <c r="I15" s="41"/>
+      <c r="J15" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="41"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="132">
+    <row r="16" spans="1:13">
+      <c r="A16" s="130">
         <v>14</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="153" t="s">
+        <v>366</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="H16" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="94" t="s">
+      <c r="I16" s="49"/>
+      <c r="J16" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="93" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="96" t="s">
+        <v>367</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>330</v>
+      </c>
+      <c r="G17" s="56" t="s">
         <v>259</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="H17" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="64" t="s">
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="63" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="130">
+    <row r="18" spans="1:25">
+      <c r="A18" s="128">
         <v>16</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="F18" s="154" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="H18" s="55" t="s">
         <v>290</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="62" t="s">
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="61" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="94" t="s">
         <v>297</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="H19" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="64" t="s">
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="63" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="133">
+    <row r="20" spans="1:25">
+      <c r="A20" s="131">
         <v>18</v>
       </c>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D20" s="147" t="s">
+        <v>308</v>
+      </c>
+      <c r="E20" s="147" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="159" t="s">
+        <v>308</v>
+      </c>
+      <c r="G20" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="H20" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="62" t="s">
+      <c r="I20" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="61" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="134">
+    <row r="21" spans="1:25">
+      <c r="A21" s="132">
         <v>19</v>
       </c>
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D21" s="148" t="s">
+        <v>308</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="G21" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="D21" s="55" t="s">
+      <c r="H21" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="64" t="s">
+      <c r="I21" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="130">
+    <row r="22" spans="1:25">
+      <c r="A22" s="128">
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D22" s="153" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="152" t="s">
+        <v>386</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="G22" s="53" t="s">
         <v>288</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="H22" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="62" t="s">
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="61" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D23" s="157" t="s">
+        <v>397</v>
+      </c>
+      <c r="E23" s="152" t="s">
+        <v>387</v>
+      </c>
+      <c r="F23" s="96" t="s">
+        <v>399</v>
+      </c>
+      <c r="G23" s="54" t="s">
         <v>287</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="H23" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="64" t="s">
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="63" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="130">
+    <row r="24" spans="1:25">
+      <c r="A24" s="128">
         <v>22</v>
       </c>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="84" t="s">
         <v>207</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D24" s="154" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="152" t="s">
+        <v>390</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="G24" s="53" t="s">
         <v>246</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="H24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="62" t="s">
+      <c r="I24" s="39"/>
+      <c r="J24" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="61" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="158" t="s">
+        <v>391</v>
+      </c>
+      <c r="F25" s="96" t="s">
+        <v>393</v>
+      </c>
+      <c r="G25" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="H25" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="64" t="s">
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="63" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="130">
+    <row r="26" spans="1:25">
+      <c r="A26" s="128">
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="D26" s="154" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="62" t="s">
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="61" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="89" t="s">
+        <v>346</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="146" t="s">
+        <v>388</v>
+      </c>
+      <c r="F27" s="146" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="81" t="s">
         <v>289</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="H27" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="64" t="s">
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="63" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="130">
-        <v>26</v>
-      </c>
-      <c r="B28" s="91" t="s">
+    <row r="28" spans="1:25">
+      <c r="A28" s="128">
+        <v>26</v>
+      </c>
+      <c r="B28" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="62" t="s">
+      <c r="I28" s="39"/>
+      <c r="J28" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M28" s="61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G29" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="H29" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="64" t="s">
+      <c r="I29" s="40"/>
+      <c r="J29" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="131">
+    <row r="30" spans="1:25">
+      <c r="A30" s="129">
         <v>28</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="D30" s="157" t="s">
+        <v>398</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="67" t="s">
+      <c r="I30" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="R30" s="52"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="130">
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" s="128">
         <v>29</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="F31" s="156" t="s">
+        <v>309</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="H31" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="39"/>
+      <c r="J31" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="R31" s="52"/>
-      <c r="U31" s="52"/>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="V31" s="51"/>
+      <c r="Y31" s="51"/>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="144" t="s">
+        <v>326</v>
+      </c>
+      <c r="D32" s="144" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="G32" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="H32" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H32" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" s="64" t="s">
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="R32" s="52"/>
-      <c r="U32" s="52"/>
-    </row>
-    <row r="33" spans="1:21">
-      <c r="A33" s="130">
+      <c r="V32" s="51"/>
+      <c r="Y32" s="51"/>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" s="128">
         <v>31</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="D33" s="71" t="s">
+      <c r="H33" s="70" t="s">
         <v>262</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="62" t="s">
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="61" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="143" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="146" t="s">
+        <v>388</v>
+      </c>
+      <c r="F34" s="146" t="s">
+        <v>300</v>
+      </c>
+      <c r="G34" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="D34" s="93" t="s">
+      <c r="H34" s="92" t="s">
         <v>217</v>
       </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="64" t="s">
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="63" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="130">
+    <row r="35" spans="1:25">
+      <c r="A35" s="128">
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="D35" s="146" t="s">
+        <v>350</v>
+      </c>
+      <c r="E35" s="143" t="s">
+        <v>377</v>
+      </c>
+      <c r="F35" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="H35" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="62" t="s">
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="61" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="140"/>
+      <c r="D36" s="140"/>
+      <c r="E36" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="154" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="54" t="s">
         <v>252</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="H36" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" s="64" t="s">
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M36" s="63" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
-      <c r="A37" s="130">
+    <row r="37" spans="1:25">
+      <c r="A37" s="128">
         <v>35</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="H37" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="62" t="s">
+      <c r="I37" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="61" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:25">
       <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G38" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="H38" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="64" t="s">
+      <c r="I38" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="S38" s="52"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="52"/>
-    </row>
-    <row r="39" spans="1:21">
-      <c r="A39" s="130">
+      <c r="W38" s="51"/>
+      <c r="X38" s="51"/>
+      <c r="Y38" s="51"/>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" s="128">
         <v>37</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="138"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="G39" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="H39" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H39" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I39" s="62" t="s">
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="S39" s="52"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="52"/>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="51"/>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="138"/>
+      <c r="D40" s="138"/>
+      <c r="E40" s="145" t="s">
+        <v>380</v>
+      </c>
+      <c r="F40" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="H40" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H40" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I40" s="64" t="s">
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="W40" s="51"/>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="51"/>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="H41" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="64" t="s">
+      <c r="I41" s="40"/>
+      <c r="J41" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-    </row>
-    <row r="42" spans="1:21">
-      <c r="A42" s="130" t="s">
+      <c r="W41" s="51"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="51"/>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="99" t="s">
+      <c r="B42" s="145" t="s">
         <v>294</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="139"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="139"/>
+      <c r="G42" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="H42" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I42" s="62" t="s">
+      <c r="I42" s="39"/>
+      <c r="J42" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52"/>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="100" t="s">
+      <c r="B43" s="98" t="s">
         <v>295</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="139"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="139"/>
+      <c r="F43" s="139"/>
+      <c r="G43" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="H43" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H43" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I43" s="64" t="s">
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M43" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
-      <c r="U43" s="52"/>
-    </row>
-    <row r="44" spans="1:21">
-      <c r="A44" s="133">
+      <c r="W43" s="51"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="51"/>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" s="131">
         <v>40</v>
       </c>
-      <c r="B44" s="81" t="s">
+      <c r="B44" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="80" t="s">
+      <c r="C44" s="139"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="54" t="s">
+      <c r="H44" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="E44" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="62" t="s">
+      <c r="I44" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="S44" s="52"/>
-      <c r="T44" s="52"/>
-      <c r="U44" s="52"/>
-    </row>
-    <row r="45" spans="1:21">
-      <c r="A45" s="133">
+      <c r="W44" s="51"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="51"/>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" s="131">
         <v>41</v>
       </c>
       <c r="B45" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="54" t="s">
+      <c r="C45" s="139"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="139"/>
+      <c r="G45" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="H45" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="E45" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="62" t="s">
+      <c r="I45" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="S45" s="52"/>
-      <c r="T45" s="52"/>
-      <c r="U45" s="52"/>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="A46" s="133">
+      <c r="W45" s="51"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="51"/>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" s="131">
         <v>42</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="138"/>
+      <c r="D46" s="138"/>
+      <c r="E46" s="138"/>
+      <c r="F46" s="138"/>
+      <c r="G46" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I46" s="62" t="s">
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M46" s="61" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
-      <c r="A47" s="133">
+    <row r="47" spans="1:25">
+      <c r="A47" s="131">
         <v>43</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="138"/>
+      <c r="D47" s="138"/>
+      <c r="E47" s="138"/>
+      <c r="F47" s="138"/>
+      <c r="G47" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="H47" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="62" t="s">
+      <c r="I47" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="61" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
-      <c r="A48" s="133">
+    <row r="48" spans="1:25">
+      <c r="A48" s="131">
         <v>44</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="138"/>
+      <c r="D48" s="138"/>
+      <c r="E48" s="138"/>
+      <c r="F48" s="138"/>
+      <c r="G48" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="H48" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="62" t="s">
+      <c r="I48" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="61" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
-      <c r="A49" s="133">
+    <row r="49" spans="1:24">
+      <c r="A49" s="131">
         <v>45</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="138"/>
+      <c r="D49" s="138"/>
+      <c r="E49" s="138"/>
+      <c r="F49" s="138"/>
+      <c r="G49" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="H49" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H49" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="62" t="s">
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M49" s="61" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
-      <c r="A50" s="134">
+    <row r="50" spans="1:24">
+      <c r="A50" s="132">
         <v>46</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="138"/>
+      <c r="D50" s="139"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="139"/>
+      <c r="G50" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="D50" s="32" t="s">
+      <c r="H50" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H50" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" s="64" t="s">
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M50" s="63" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
-      <c r="A51" s="133">
+    <row r="51" spans="1:24">
+      <c r="A51" s="131">
         <v>47</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="138"/>
+      <c r="D51" s="138"/>
+      <c r="E51" s="138"/>
+      <c r="F51" s="138"/>
+      <c r="G51" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="H51" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H51" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I51" s="62" t="s">
+      <c r="I51" s="39"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L51" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M51" s="61" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:24">
       <c r="A52" s="2">
         <v>48</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="138"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="139"/>
+      <c r="F52" s="139"/>
+      <c r="G52" s="54" t="s">
         <v>266</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="H52" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H52" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I52" s="64" t="s">
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M52" s="63" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
-      <c r="A53" s="130">
+    <row r="53" spans="1:24">
+      <c r="A53" s="128">
         <v>49</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="59" t="s">
+      <c r="C53" s="138"/>
+      <c r="D53" s="138"/>
+      <c r="E53" s="138"/>
+      <c r="F53" s="138"/>
+      <c r="G53" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="D53" s="52" t="s">
+      <c r="H53" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="E53" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="62" t="s">
+      <c r="I53" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J53" s="39"/>
+      <c r="K53" s="39"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:24">
       <c r="A54" s="2">
         <v>50</v>
       </c>
-      <c r="B54" s="87" t="s">
+      <c r="B54" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="138"/>
+      <c r="D54" s="138"/>
+      <c r="E54" s="138"/>
+      <c r="F54" s="138"/>
+      <c r="G54" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="H54" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E54" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="64" t="s">
+      <c r="I54" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="K54" s="126" t="s">
+      <c r="O54" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="L54" s="102"/>
-      <c r="M54" s="102"/>
-      <c r="N54" s="102"/>
-      <c r="O54" s="80"/>
-      <c r="S54" t="s">
+      <c r="P54" s="100"/>
+      <c r="Q54" s="100"/>
+      <c r="R54" s="100"/>
+      <c r="S54" s="79"/>
+      <c r="W54" t="s">
         <v>310</v>
       </c>
-      <c r="T54">
+      <c r="X54">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="17" thickBot="1">
-      <c r="A55" s="132">
+    <row r="55" spans="1:24" ht="17" thickBot="1">
+      <c r="A55" s="130">
         <v>51</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="138"/>
+      <c r="D55" s="138"/>
+      <c r="E55" s="138"/>
+      <c r="F55" s="138"/>
+      <c r="G55" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="D55" s="49" t="s">
+      <c r="H55" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="H55" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="I55" s="62" t="s">
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="M55" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="K55" s="127" t="s">
+      <c r="O55" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="L55" s="145" t="s">
+      <c r="P55" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="M55" s="145"/>
-      <c r="N55" s="79" t="s">
+      <c r="Q55" s="170"/>
+      <c r="R55" s="78" t="s">
         <v>165</v>
       </c>
-      <c r="O55" s="128" t="s">
+      <c r="S55" s="126" t="s">
         <v>169</v>
       </c>
-      <c r="Q55" s="52"/>
-      <c r="S55" t="s">
+      <c r="U55" s="51"/>
+      <c r="W55" t="s">
         <v>311</v>
       </c>
-      <c r="T55">
+      <c r="X55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
-      <c r="A56" s="130">
+    <row r="56" spans="1:24">
+      <c r="A56" s="128">
         <v>52</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="138"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="138"/>
+      <c r="G56" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="H56" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H56" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" s="62" t="s">
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L56" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M56" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="K56" s="129" t="s">
+      <c r="O56" s="127" t="s">
         <v>155</v>
       </c>
-      <c r="L56" s="146" t="s">
+      <c r="P56" s="171" t="s">
         <v>158</v>
       </c>
-      <c r="M56" s="146"/>
-      <c r="N56" s="110" t="s">
+      <c r="Q56" s="171"/>
+      <c r="R56" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="O56" s="112" t="s">
+      <c r="S56" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="Q56" s="52"/>
-      <c r="S56" t="s">
+      <c r="U56" s="51"/>
+      <c r="W56" t="s">
         <v>312</v>
       </c>
-      <c r="T56">
+      <c r="X56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
-      <c r="A57" s="130">
+    <row r="57" spans="1:24">
+      <c r="A57" s="128">
         <v>53</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="138"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="138"/>
+      <c r="F57" s="138"/>
+      <c r="G57" s="30" t="s">
         <v>269</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="H57" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="H57" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I57" s="62" t="s">
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="L57" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M57" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="K57" s="129" t="s">
+      <c r="O57" s="127" t="s">
         <v>156</v>
       </c>
-      <c r="L57" s="147" t="s">
+      <c r="P57" s="172" t="s">
         <v>306</v>
       </c>
-      <c r="M57" s="147"/>
-      <c r="N57" s="110"/>
-      <c r="O57" s="54"/>
-      <c r="Q57" s="52"/>
-      <c r="R57" s="53"/>
-      <c r="S57" s="53" t="s">
+      <c r="Q57" s="172"/>
+      <c r="R57" s="108"/>
+      <c r="S57" s="53"/>
+      <c r="U57" s="51"/>
+      <c r="V57" s="52"/>
+      <c r="W57" s="52" t="s">
         <v>313</v>
       </c>
-      <c r="T57">
+      <c r="X57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
-      <c r="A58" s="130">
+    <row r="58" spans="1:24">
+      <c r="A58" s="128">
         <v>54</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="138"/>
+      <c r="D58" s="138"/>
+      <c r="E58" s="138"/>
+      <c r="F58" s="138"/>
+      <c r="G58" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="H58" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H58" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I58" s="62" t="s">
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L58" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M58" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="K58" s="109" t="s">
+      <c r="O58" s="107" t="s">
         <v>157</v>
       </c>
-      <c r="L58" s="148" t="s">
+      <c r="P58" s="173" t="s">
         <v>305</v>
       </c>
-      <c r="M58" s="148"/>
-      <c r="N58" s="72" t="s">
+      <c r="Q58" s="173"/>
+      <c r="R58" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="O58" s="112" t="s">
+      <c r="S58" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="S58" s="53" t="s">
+      <c r="W58" s="52" t="s">
         <v>316</v>
       </c>
-      <c r="T58">
+      <c r="X58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:24">
       <c r="A59" s="2">
         <v>55</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="138"/>
+      <c r="D59" s="138"/>
+      <c r="E59" s="138"/>
+      <c r="F59" s="138"/>
+      <c r="G59" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="H59" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H59" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I59" s="64" t="s">
+      <c r="I59" s="40"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M59" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="K59" s="109" t="s">
+      <c r="O59" s="107" t="s">
         <v>159</v>
       </c>
-      <c r="L59" s="148" t="s">
+      <c r="P59" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="M59" s="148"/>
-      <c r="N59" s="72" t="s">
+      <c r="Q59" s="173"/>
+      <c r="R59" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="O59" s="112" t="s">
+      <c r="S59" s="110" t="s">
         <v>170</v>
       </c>
-      <c r="T59">
-        <f>SUM(T54:T58)</f>
+      <c r="X59">
+        <f>SUM(X54:X58)</f>
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
-      <c r="A60" s="130">
+    <row r="60" spans="1:24">
+      <c r="A60" s="128">
         <v>56</v>
       </c>
-      <c r="B60" s="89" t="s">
+      <c r="B60" s="88" t="s">
         <v>284</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="138"/>
+      <c r="D60" s="138"/>
+      <c r="E60" s="138"/>
+      <c r="F60" s="138"/>
+      <c r="G60" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="H60" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H60" s="40"/>
-      <c r="I60" s="62" t="s">
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L60" s="39"/>
+      <c r="M60" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="K60" s="113" t="s">
+      <c r="O60" s="111" t="s">
         <v>162</v>
       </c>
-      <c r="L60" s="149" t="s">
+      <c r="P60" s="174" t="s">
         <v>307</v>
       </c>
-      <c r="M60" s="149"/>
-      <c r="N60" s="73"/>
-      <c r="O60" s="57"/>
-    </row>
-    <row r="61" spans="1:20">
+      <c r="Q60" s="174"/>
+      <c r="R60" s="72"/>
+      <c r="S60" s="56"/>
+    </row>
+    <row r="61" spans="1:24">
       <c r="A61" s="2">
         <v>57</v>
       </c>
-      <c r="B61" s="90" t="s">
+      <c r="B61" s="89" t="s">
         <v>285</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="138"/>
+      <c r="D61" s="138"/>
+      <c r="E61" s="138"/>
+      <c r="F61" s="138"/>
+      <c r="G61" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="H61" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H61" s="41"/>
-      <c r="I61" s="64" t="s">
+      <c r="I61" s="40"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L61" s="40"/>
+      <c r="M61" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="K61" s="66"/>
-      <c r="L61" s="66"/>
-      <c r="M61" s="66"/>
-    </row>
-    <row r="62" spans="1:20" s="1" customFormat="1">
-      <c r="A62" s="132" t="s">
+      <c r="O61" s="65"/>
+      <c r="P61" s="65"/>
+      <c r="Q61" s="65"/>
+    </row>
+    <row r="62" spans="1:24" s="1" customFormat="1">
+      <c r="A62" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="B62" s="84" t="s">
+      <c r="B62" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="31" t="s">
-        <v>280</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="50"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="63" t="s">
+      <c r="C62" s="138"/>
+      <c r="D62" s="138"/>
+      <c r="E62" s="138"/>
+      <c r="F62" s="138"/>
+      <c r="G62" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="K62" s="105" t="s">
+      <c r="O62" s="103" t="s">
         <v>189</v>
       </c>
-      <c r="L62" s="106"/>
-      <c r="M62" s="104"/>
-      <c r="O62" s="105" t="s">
+      <c r="P62" s="104"/>
+      <c r="Q62" s="102"/>
+      <c r="S62" s="103" t="s">
         <v>176</v>
       </c>
-      <c r="P62" s="106"/>
-      <c r="Q62" s="104"/>
-    </row>
-    <row r="63" spans="1:20" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="T62" s="104"/>
+      <c r="U62" s="102"/>
+    </row>
+    <row r="63" spans="1:24" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A63" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="87" t="s">
+      <c r="B63" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="D63" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="41"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="69" t="s">
+      <c r="C63" s="138"/>
+      <c r="D63" s="138"/>
+      <c r="E63" s="138"/>
+      <c r="F63" s="138"/>
+      <c r="G63" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="H63" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="40"/>
+      <c r="K63" s="40"/>
+      <c r="L63" s="44"/>
+      <c r="M63" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="K63" s="107" t="s">
+      <c r="O63" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="L63" s="78" t="s">
+      <c r="P63" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="M63" s="108" t="s">
+      <c r="Q63" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="O63" s="107" t="s">
+      <c r="S63" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="P63" s="78" t="s">
+      <c r="T63" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="Q63" s="108" t="s">
+      <c r="U63" s="106" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" s="1" customFormat="1">
-      <c r="A64" s="135" t="s">
+    <row r="64" spans="1:24" s="1" customFormat="1">
+      <c r="A64" s="133" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="138"/>
+      <c r="D64" s="138"/>
+      <c r="E64" s="138"/>
+      <c r="F64" s="138"/>
+      <c r="G64" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="D64" s="38" t="s">
+      <c r="H64" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E64" s="31"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H64" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="I64" s="63" t="s">
+      <c r="I64" s="30"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L64" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="M64" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="K64" s="109" t="s">
+      <c r="O64" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="L64" s="110" t="s">
+      <c r="P64" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="M64" s="111">
+      <c r="Q64" s="109">
         <v>2</v>
       </c>
-      <c r="O64" s="109" t="s">
+      <c r="S64" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="P64" s="72" t="s">
+      <c r="T64" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="Q64" s="112">
+      <c r="U64" s="110">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="1" customFormat="1">
-      <c r="A65" s="134" t="s">
+    <row r="65" spans="1:21" s="1" customFormat="1">
+      <c r="A65" s="132" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="138"/>
+      <c r="D65" s="138"/>
+      <c r="E65" s="138"/>
+      <c r="F65" s="138"/>
+      <c r="G65" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="D65" s="39" t="s">
+      <c r="H65" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E65" s="41"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H65" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I65" s="69" t="s">
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="M65" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="K65" s="109" t="s">
+      <c r="O65" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="L65" s="72" t="s">
+      <c r="P65" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="M65" s="112">
+      <c r="Q65" s="110">
         <v>10</v>
       </c>
-      <c r="O65" s="109" t="s">
+      <c r="S65" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="P65" s="72" t="s">
+      <c r="T65" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="Q65" s="120">
+      <c r="U65" s="118">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
-      <c r="A66" s="131" t="s">
+    <row r="66" spans="1:21">
+      <c r="A66" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="138"/>
+      <c r="D66" s="138"/>
+      <c r="E66" s="138"/>
+      <c r="F66" s="138"/>
+      <c r="G66" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D66" s="35" t="s">
+      <c r="H66" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="I66" s="67" t="s">
+      <c r="I66" s="41"/>
+      <c r="J66" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K66" s="41"/>
+      <c r="L66" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="M66" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="K66" s="113" t="s">
+      <c r="O66" s="111" t="s">
         <v>174</v>
       </c>
-      <c r="L66" s="74" t="s">
+      <c r="P66" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="M66" s="114">
-        <v>26</v>
-      </c>
-      <c r="O66" s="113" t="s">
+      <c r="Q66" s="112">
+        <v>26</v>
+      </c>
+      <c r="S66" s="111" t="s">
         <v>177</v>
       </c>
-      <c r="P66" s="75" t="s">
+      <c r="T66" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="Q66" s="116" t="s">
+      <c r="U66" s="114" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
-      <c r="A67" s="131" t="s">
+    <row r="67" spans="1:21">
+      <c r="A67" s="129" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="H67" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="I67" s="64" t="s">
+      <c r="I67" s="41"/>
+      <c r="J67" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K67" s="41"/>
+      <c r="L67" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="M67" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="K67" s="109" t="s">
+      <c r="O67" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="L67" s="72" t="s">
+      <c r="P67" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="M67" s="115">
+      <c r="Q67" s="113">
         <v>6</v>
       </c>
-      <c r="O67" s="121" t="s">
+      <c r="S67" s="119" t="s">
         <v>178</v>
       </c>
-      <c r="P67" s="52" t="s">
+      <c r="T67" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="Q67" s="54" t="s">
+      <c r="U67" s="53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
-      <c r="A68" s="136"/>
+    <row r="68" spans="1:21">
+      <c r="A68" s="134"/>
       <c r="B68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="65"/>
-      <c r="K68" s="113" t="s">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="64"/>
+      <c r="O68" s="111" t="s">
         <v>190</v>
       </c>
-      <c r="L68" s="74" t="s">
+      <c r="P68" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="M68" s="116">
+      <c r="Q68" s="114">
         <v>9</v>
       </c>
-      <c r="O68" s="122" t="s">
+      <c r="S68" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="P68" s="73" t="s">
+      <c r="T68" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="Q68" s="116" t="s">
+      <c r="U68" s="114" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
-      <c r="A69" s="136"/>
-      <c r="B69" s="101" t="s">
+    <row r="69" spans="1:21">
+      <c r="A69" s="134"/>
+      <c r="B69" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="102"/>
-      <c r="D69" s="102"/>
-      <c r="E69" s="102"/>
-      <c r="F69" s="102"/>
-      <c r="G69" s="102"/>
-      <c r="H69" s="103"/>
-      <c r="I69" s="104"/>
-      <c r="K69" s="109" t="s">
+      <c r="C69" s="137"/>
+      <c r="D69" s="137"/>
+      <c r="E69" s="137"/>
+      <c r="F69" s="137"/>
+      <c r="G69" s="100"/>
+      <c r="H69" s="100"/>
+      <c r="I69" s="100"/>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+      <c r="L69" s="101"/>
+      <c r="M69" s="102"/>
+      <c r="O69" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="L69" s="72" t="s">
+      <c r="P69" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="M69" s="111">
+      <c r="Q69" s="109">
         <v>20</v>
       </c>
-      <c r="O69" s="123" t="s">
+      <c r="S69" s="121" t="s">
         <v>179</v>
       </c>
-      <c r="P69" s="76" t="s">
+      <c r="T69" s="75" t="s">
         <v>185</v>
       </c>
-      <c r="Q69" s="124" t="s">
+      <c r="U69" s="122" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="16" customHeight="1">
-      <c r="A70" s="136"/>
-      <c r="B70" s="139" t="s">
+    <row r="70" spans="1:21" ht="16" customHeight="1">
+      <c r="A70" s="134"/>
+      <c r="B70" s="164" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="140"/>
-      <c r="D70" s="140"/>
-      <c r="E70" s="140"/>
-      <c r="F70" s="140"/>
-      <c r="G70" s="140"/>
-      <c r="H70" s="140"/>
-      <c r="I70" s="141"/>
-      <c r="K70" s="113" t="s">
+      <c r="C70" s="165"/>
+      <c r="D70" s="165"/>
+      <c r="E70" s="165"/>
+      <c r="F70" s="165"/>
+      <c r="G70" s="165"/>
+      <c r="H70" s="165"/>
+      <c r="I70" s="165"/>
+      <c r="J70" s="165"/>
+      <c r="K70" s="165"/>
+      <c r="L70" s="165"/>
+      <c r="M70" s="166"/>
+      <c r="O70" s="111" t="s">
         <v>191</v>
       </c>
-      <c r="L70" s="74" t="s">
+      <c r="P70" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="M70" s="116">
+      <c r="Q70" s="114">
         <v>23</v>
       </c>
-      <c r="O70" s="122" t="s">
+      <c r="S70" s="120" t="s">
         <v>184</v>
       </c>
-      <c r="P70" s="73" t="s">
+      <c r="T70" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="Q70" s="116" t="s">
+      <c r="U70" s="114" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
-      <c r="B71" s="139"/>
-      <c r="C71" s="140"/>
-      <c r="D71" s="140"/>
-      <c r="E71" s="140"/>
-      <c r="F71" s="140"/>
-      <c r="G71" s="140"/>
-      <c r="H71" s="140"/>
-      <c r="I71" s="141"/>
-      <c r="K71" s="109" t="s">
+    <row r="71" spans="1:21">
+      <c r="B71" s="164"/>
+      <c r="C71" s="165"/>
+      <c r="D71" s="165"/>
+      <c r="E71" s="165"/>
+      <c r="F71" s="165"/>
+      <c r="G71" s="165"/>
+      <c r="H71" s="165"/>
+      <c r="I71" s="165"/>
+      <c r="J71" s="165"/>
+      <c r="K71" s="165"/>
+      <c r="L71" s="165"/>
+      <c r="M71" s="166"/>
+      <c r="O71" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="L71" s="72" t="s">
+      <c r="P71" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="M71" s="111">
+      <c r="Q71" s="109">
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
-      <c r="A72" s="136"/>
-      <c r="B72" s="139"/>
-      <c r="C72" s="140"/>
-      <c r="D72" s="140"/>
-      <c r="E72" s="140"/>
-      <c r="F72" s="140"/>
-      <c r="G72" s="140"/>
-      <c r="H72" s="140"/>
-      <c r="I72" s="141"/>
-      <c r="K72" s="113" t="s">
+    <row r="72" spans="1:21">
+      <c r="A72" s="134"/>
+      <c r="B72" s="164"/>
+      <c r="C72" s="165"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
+      <c r="F72" s="165"/>
+      <c r="G72" s="165"/>
+      <c r="H72" s="165"/>
+      <c r="I72" s="165"/>
+      <c r="J72" s="165"/>
+      <c r="K72" s="165"/>
+      <c r="L72" s="165"/>
+      <c r="M72" s="166"/>
+      <c r="O72" s="111" t="s">
         <v>192</v>
       </c>
-      <c r="L72" s="74" t="s">
+      <c r="P72" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="M72" s="116">
+      <c r="Q72" s="114">
         <v>22</v>
       </c>
-      <c r="O72" s="105" t="s">
+      <c r="S72" s="103" t="s">
         <v>181</v>
       </c>
-      <c r="P72" s="106"/>
-      <c r="Q72" s="104"/>
-    </row>
-    <row r="73" spans="1:17" ht="17" thickBot="1">
-      <c r="B73" s="139"/>
-      <c r="C73" s="140"/>
-      <c r="D73" s="140"/>
-      <c r="E73" s="140"/>
-      <c r="F73" s="140"/>
-      <c r="G73" s="140"/>
-      <c r="H73" s="140"/>
-      <c r="I73" s="141"/>
-      <c r="K73" s="117" t="s">
+      <c r="T72" s="104"/>
+      <c r="U72" s="102"/>
+    </row>
+    <row r="73" spans="1:21" ht="17" thickBot="1">
+      <c r="B73" s="164"/>
+      <c r="C73" s="165"/>
+      <c r="D73" s="165"/>
+      <c r="E73" s="165"/>
+      <c r="F73" s="165"/>
+      <c r="G73" s="165"/>
+      <c r="H73" s="165"/>
+      <c r="I73" s="165"/>
+      <c r="J73" s="165"/>
+      <c r="K73" s="165"/>
+      <c r="L73" s="165"/>
+      <c r="M73" s="166"/>
+      <c r="O73" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="L73" s="77" t="s">
+      <c r="P73" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="M73" s="118">
+      <c r="Q73" s="116">
         <v>15</v>
       </c>
-      <c r="O73" s="107" t="s">
+      <c r="S73" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="P73" s="78" t="s">
+      <c r="T73" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="Q73" s="108" t="s">
+      <c r="U73" s="106" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
-      <c r="A74" s="136"/>
-      <c r="B74" s="139"/>
-      <c r="C74" s="140"/>
-      <c r="D74" s="140"/>
-      <c r="E74" s="140"/>
-      <c r="F74" s="140"/>
-      <c r="G74" s="140"/>
-      <c r="H74" s="140"/>
-      <c r="I74" s="141"/>
-      <c r="K74" s="113" t="s">
+    <row r="74" spans="1:21">
+      <c r="A74" s="134"/>
+      <c r="B74" s="164"/>
+      <c r="C74" s="165"/>
+      <c r="D74" s="165"/>
+      <c r="E74" s="165"/>
+      <c r="F74" s="165"/>
+      <c r="G74" s="165"/>
+      <c r="H74" s="165"/>
+      <c r="I74" s="165"/>
+      <c r="J74" s="165"/>
+      <c r="K74" s="165"/>
+      <c r="L74" s="165"/>
+      <c r="M74" s="166"/>
+      <c r="O74" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="L74" s="74" t="s">
+      <c r="P74" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="M74" s="119">
+      <c r="Q74" s="117">
         <v>45</v>
       </c>
-      <c r="O74" s="109" t="s">
+      <c r="S74" s="107" t="s">
         <v>187</v>
       </c>
-      <c r="P74" s="72" t="s">
+      <c r="T74" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="Q74" s="112">
+      <c r="U74" s="110">
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
-      <c r="A75" s="136"/>
-      <c r="B75" s="139"/>
-      <c r="C75" s="140"/>
-      <c r="D75" s="140"/>
-      <c r="E75" s="140"/>
-      <c r="F75" s="140"/>
-      <c r="G75" s="140"/>
-      <c r="H75" s="140"/>
-      <c r="I75" s="141"/>
-      <c r="O75" s="113" t="s">
+    <row r="75" spans="1:21">
+      <c r="A75" s="134"/>
+      <c r="B75" s="164"/>
+      <c r="C75" s="165"/>
+      <c r="D75" s="165"/>
+      <c r="E75" s="165"/>
+      <c r="F75" s="165"/>
+      <c r="G75" s="165"/>
+      <c r="H75" s="165"/>
+      <c r="I75" s="165"/>
+      <c r="J75" s="165"/>
+      <c r="K75" s="165"/>
+      <c r="L75" s="165"/>
+      <c r="M75" s="166"/>
+      <c r="S75" s="111" t="s">
         <v>187</v>
       </c>
-      <c r="P75" s="74" t="s">
+      <c r="T75" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="Q75" s="125">
+      <c r="U75" s="123">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
-      <c r="B76" s="139"/>
-      <c r="C76" s="140"/>
-      <c r="D76" s="140"/>
-      <c r="E76" s="140"/>
-      <c r="F76" s="140"/>
-      <c r="G76" s="140"/>
-      <c r="H76" s="140"/>
-      <c r="I76" s="141"/>
-      <c r="O76" s="113" t="s">
+    <row r="76" spans="1:21">
+      <c r="B76" s="164"/>
+      <c r="C76" s="165"/>
+      <c r="D76" s="165"/>
+      <c r="E76" s="165"/>
+      <c r="F76" s="165"/>
+      <c r="G76" s="165"/>
+      <c r="H76" s="165"/>
+      <c r="I76" s="165"/>
+      <c r="J76" s="165"/>
+      <c r="K76" s="165"/>
+      <c r="L76" s="165"/>
+      <c r="M76" s="166"/>
+      <c r="S76" s="111" t="s">
         <v>188</v>
       </c>
-      <c r="P76" s="75" t="s">
+      <c r="T76" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="Q76" s="125">
+      <c r="U76" s="123">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
-      <c r="B77" s="139"/>
-      <c r="C77" s="140"/>
-      <c r="D77" s="140"/>
-      <c r="E77" s="140"/>
-      <c r="F77" s="140"/>
-      <c r="G77" s="140"/>
-      <c r="H77" s="140"/>
-      <c r="I77" s="141"/>
-    </row>
-    <row r="78" spans="1:17">
-      <c r="B78" s="142"/>
-      <c r="C78" s="143"/>
-      <c r="D78" s="143"/>
-      <c r="E78" s="143"/>
-      <c r="F78" s="143"/>
-      <c r="G78" s="143"/>
-      <c r="H78" s="143"/>
-      <c r="I78" s="144"/>
+    <row r="77" spans="1:21">
+      <c r="B77" s="164"/>
+      <c r="C77" s="165"/>
+      <c r="D77" s="165"/>
+      <c r="E77" s="165"/>
+      <c r="F77" s="165"/>
+      <c r="G77" s="165"/>
+      <c r="H77" s="165"/>
+      <c r="I77" s="165"/>
+      <c r="J77" s="165"/>
+      <c r="K77" s="165"/>
+      <c r="L77" s="165"/>
+      <c r="M77" s="166"/>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="B78" s="167"/>
+      <c r="C78" s="168"/>
+      <c r="D78" s="168"/>
+      <c r="E78" s="168"/>
+      <c r="F78" s="168"/>
+      <c r="G78" s="168"/>
+      <c r="H78" s="168"/>
+      <c r="I78" s="168"/>
+      <c r="J78" s="168"/>
+      <c r="K78" s="168"/>
+      <c r="L78" s="168"/>
+      <c r="M78" s="169"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="138" t="s">
+      <c r="A81" s="136" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B70:I78"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="B70:M78"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="P60:Q60"/>
   </mergeCells>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0.196850393700787" header="0.196850393700787" footer="3.9370078740157501E-2"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" cellComments="asDisplayed" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>